<commit_message>
Atualização da Planilha de Cronograma, inserindo novos itens (faltam ajustes nas macros)
</commit_message>
<xml_diff>
--- a/Documentacao/GERENCIA/Cronograma.xlsx
+++ b/Documentacao/GERENCIA/Cronograma.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22204"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24777497-FD4E-4BBF-9FDC-96072F99A9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026DF126-761F-6B4F-BBA1-4F0374D9AE88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3560" yWindow="3200" windowWidth="27300" windowHeight="13960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,8 @@
     <definedName name="PeriodInPlan">Projeto!A$8=MEDIAN(Projeto!A$8,Projeto!$C1,Projeto!$C1+Projeto!$D1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*(Projeto!$C1&gt;0)</definedName>
   </definedNames>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>PLANEJAMENTO</t>
   </si>
@@ -159,12 +153,6 @@
     <t>Plano de projeto</t>
   </si>
   <si>
-    <t>Blog</t>
-  </si>
-  <si>
-    <t>GitHub</t>
-  </si>
-  <si>
     <t>Casos de uso</t>
   </si>
   <si>
@@ -174,12 +162,6 @@
     <t>Testes dos equipamentos</t>
   </si>
   <si>
-    <t>Inicio da programação</t>
-  </si>
-  <si>
-    <t>Desenvolvimento/programação</t>
-  </si>
-  <si>
     <t>Ajustes e correções</t>
   </si>
   <si>
@@ -190,13 +172,43 @@
   </si>
   <si>
     <t>Documentação final</t>
+  </si>
+  <si>
+    <t>Preparação e Montagem inicial dos dispositivos</t>
+  </si>
+  <si>
+    <t>Outros digramas UML</t>
+  </si>
+  <si>
+    <t>Inicio da programação / Blynk / Circuitos</t>
+  </si>
+  <si>
+    <t>Testes</t>
+  </si>
+  <si>
+    <t>Programação / Blynk / Adaptação dos Circuitos</t>
+  </si>
+  <si>
+    <t>Blog - Criação e Atualização</t>
+  </si>
+  <si>
+    <t>GitHub - Criação e Atualização</t>
+  </si>
+  <si>
+    <t>Preparação da Entrega 1</t>
+  </si>
+  <si>
+    <t>Preparação da Entrega 2</t>
+  </si>
+  <si>
+    <t>Preparação da Entrega 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -486,13 +498,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Título 1" xfId="1" builtinId="16" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="26">
     <dxf>
@@ -1166,29 +1178,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AS20"/>
+  <dimension ref="B2:AS26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
-    <col min="9" max="12" width="2.75" style="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="2.6640625" style="1"/>
     <col min="13" max="13" width="3.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="3.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="28" width="2.75" style="1"/>
+    <col min="14" max="14" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="28" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:45" ht="15">
+    <row r="2" spans="2:45" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1210,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="2:45" ht="21" customHeight="1">
+    <row r="3" spans="2:45" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -1213,7 +1225,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1241,7 +1253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:45" ht="18.75" customHeight="1">
+    <row r="4" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1249,7 +1261,7 @@
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="2:45">
+    <row r="5" spans="2:45" x14ac:dyDescent="0.25">
       <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1282,7 +1294,7 @@
       <c r="AF5" s="19"/>
       <c r="AG5" s="19"/>
     </row>
-    <row r="6" spans="2:45" ht="15">
+    <row r="6" spans="2:45" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="23" t="s">
         <v>8</v>
@@ -1303,7 +1315,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="2:45" ht="13.5" customHeight="1">
+    <row r="7" spans="2:45" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1318,7 +1330,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:45" ht="15.75" customHeight="1">
+    <row r="8" spans="2:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1438,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:45" ht="18.75" customHeight="1">
+    <row r="9" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
         <v>15</v>
       </c>
@@ -1458,49 +1470,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:45" ht="18.75" customHeight="1">
+    <row r="10" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="18" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C10" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" s="15">
-        <v>3</v>
-      </c>
-      <c r="E10" s="15">
-        <v>4</v>
-      </c>
-      <c r="F10" s="15">
-        <v>3</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:45" ht="18.75" customHeight="1">
+    <row r="11" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C11" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="15">
-        <v>2</v>
-      </c>
-      <c r="E11" s="15">
-        <v>2</v>
-      </c>
-      <c r="F11" s="15">
-        <v>2</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:45" ht="18.75" customHeight="1">
+    <row r="12" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="15">
         <v>5</v>
@@ -1518,139 +1522,237 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:45" ht="18.95" customHeight="1">
+    <row r="13" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C13" s="15">
+        <v>6</v>
+      </c>
+      <c r="D13" s="15">
         <v>8</v>
       </c>
-      <c r="D13" s="21">
-        <v>5</v>
-      </c>
       <c r="E13" s="15">
+        <v>6</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="15">
+        <v>7</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15">
+        <v>7</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15">
+        <v>14</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="2:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="15">
+        <v>21</v>
+      </c>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15">
+        <v>21</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1</v>
+      </c>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="15">
+        <v>15</v>
+      </c>
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="16">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="15">
         <v>8</v>
       </c>
-      <c r="F13" s="21">
-        <v>5</v>
-      </c>
-      <c r="G13" s="16">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="14" spans="2:45" ht="18.95" customHeight="1">
-      <c r="B14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="15">
-        <v>11</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="D18" s="15">
         <v>4</v>
       </c>
-      <c r="E14" s="15">
-        <v>11</v>
-      </c>
-      <c r="F14" s="15">
-        <v>4</v>
-      </c>
-      <c r="G14" s="16">
+      <c r="E18" s="15">
+        <v>8</v>
+      </c>
+      <c r="F18" s="15">
+        <v>2</v>
+      </c>
+      <c r="G18" s="16">
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="2:45" ht="18.95" customHeight="1">
-      <c r="B15" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="15">
-        <v>15</v>
-      </c>
-      <c r="D15" s="15">
-        <v>2</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:45" ht="18.95" customHeight="1">
-      <c r="B16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="15">
-        <v>17</v>
-      </c>
-      <c r="D16" s="15">
-        <v>7</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="18.95" customHeight="1">
-      <c r="B17" s="18" t="s">
+    <row r="19" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="15">
-        <v>22</v>
-      </c>
-      <c r="D17" s="15">
-        <v>7</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="18.95" customHeight="1">
-      <c r="B18" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="15">
-        <v>24</v>
-      </c>
-      <c r="D18" s="15">
-        <v>5</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="18.95" customHeight="1">
-      <c r="B19" s="18" t="s">
-        <v>25</v>
-      </c>
       <c r="C19" s="15">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D19" s="15">
         <v>2</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="18.95" customHeight="1">
+      <c r="E19" s="15">
+        <v>9</v>
+      </c>
+      <c r="F19" s="15">
+        <v>2</v>
+      </c>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="15">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D20" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="15">
+        <v>17</v>
+      </c>
+      <c r="D21" s="15">
+        <v>11</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="15">
+        <v>27</v>
+      </c>
+      <c r="D22" s="15">
+        <v>2</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="15">
+        <v>29</v>
+      </c>
+      <c r="D23" s="15">
+        <v>4</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="15">
+        <v>33</v>
+      </c>
+      <c r="D24" s="15">
+        <v>2</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="15">
+        <v>29</v>
+      </c>
+      <c r="D25" s="15">
+        <v>6</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="15">
+        <v>32</v>
+      </c>
+      <c r="D26" s="15">
+        <v>6</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1663,7 +1765,7 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:AS9 I12:AS20">
+  <conditionalFormatting sqref="I9:AS9 I12:AS26">
     <cfRule type="expression" dxfId="25" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1689,7 +1791,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:AS21">
+  <conditionalFormatting sqref="B27:AS27">
     <cfRule type="expression" dxfId="17" priority="18">
       <formula>TRUE</formula>
     </cfRule>
@@ -1772,5 +1874,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{034D67AC-589E-4C00-9B1A-F2A41167CA08}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{034D67AC-589E-4C00-9B1A-F2A41167CA08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>